<commit_message>
added web app sample
</commit_message>
<xml_diff>
--- a/slides/Book1.xlsx
+++ b/slides/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamie\Dropbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamie/Documents/GitHub/AzureTradeoffs/slides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1785E52A-D656-4755-90DB-FFC8F9FAE46E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7B26C8-B157-3643-87AB-DA6B8E6E8AD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{0F04EAE2-F429-4719-8896-262EDF60BCAA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22440" xr2:uid="{0F04EAE2-F429-4719-8896-262EDF60BCAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -307,99 +307,85 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$20:$P$20</c:f>
-              <c:strCache>
-                <c:ptCount val="15"/>
+            <c:numRef>
+              <c:f>Sheet1!$C$20:$M$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>Millions of requests</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$21:$P$21</c:f>
+              <c:f>Sheet1!$C$21:$M$21</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>1.5999999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.7999999999999989</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>17.999999999999996</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>26.2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>34.4</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>42.6</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>50.8</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>58.999999999999993</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>67.199999999999989</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>75.399999999999991</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>83.6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>91.8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>108.19999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -413,7 +399,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$B$24</c:f>
@@ -450,64 +436,53 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$20:$P$20</c:f>
-              <c:strCache>
-                <c:ptCount val="15"/>
+            <c:numRef>
+              <c:f>Sheet1!$C$20:$M$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>Millions of requests</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$24:$P$24</c:f>
+              <c:f>Sheet1!$C$24:$M$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>74.400000000000006</c:v>
                 </c:pt>
@@ -539,9 +514,6 @@
                   <c:v>74.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>74.400000000000006</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>74.400000000000006</c:v>
                 </c:pt>
               </c:numCache>
@@ -566,173 +538,7 @@
         <c:smooth val="0"/>
         <c:axId val="587754168"/>
         <c:axId val="577716304"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredLineSeries>
-              <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="1"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$20</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>Millions of requests</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="28575" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent2"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent2"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent2"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:cat>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$20:$P$20</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="15"/>
-                      <c:pt idx="0">
-                        <c:v>Millions of requests</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>1</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>2</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>3</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>4</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>5</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>6</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>7</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>8</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>9</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>10</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>11</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>12</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>13</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>14</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:cat>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$E$20:$P$20</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="12"/>
-                      <c:pt idx="0">
-                        <c:v>3</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>4</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>5</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>6</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>7</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>8</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>9</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>10</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>11</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>12</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>13</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>14</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-EED3-4581-B054-E53068305F9A}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredLineSeries>
-          </c:ext>
-        </c:extLst>
+        <c:extLst/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="587754168"/>
@@ -4168,26 +3974,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF4A6AE-7AEF-4A03-91C5-25DD83BB1920}">
   <dimension ref="B4:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C4">
         <v>74.400000000000006</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -4245,7 +4051,7 @@
         <v>14000000</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -4292,7 +4098,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -4339,7 +4145,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -4400,7 +4206,7 @@
         <v>20600000</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -4461,7 +4267,7 @@
         <v>329.59999999999997</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>5</v>
       </c>
@@ -4522,7 +4328,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C16" s="2">
         <f t="shared" ref="C16:D16" si="6">C14+C13</f>
         <v>17.599999999999998</v>
@@ -4580,7 +4386,7 @@
         <v>332.2</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C18">
         <f>60*60*24*31</f>
         <v>2678400</v>
@@ -4594,7 +4400,7 @@
         <v>2678400</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C19">
         <f>C20*1000000/$E$18</f>
         <v>0.37335722819593786</v>
@@ -4652,7 +4458,7 @@
         <v>5.2270011947431305</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>6</v>
       </c>
@@ -4710,7 +4516,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>25</v>
       </c>
@@ -4757,7 +4563,7 @@
         <v>108.19999999999999</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>26</v>
       </c>
@@ -4804,7 +4610,7 @@
         <v>220.2</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>27</v>
       </c>
@@ -4851,7 +4657,7 @@
         <v>332.2</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>7</v>
       </c>
@@ -4898,7 +4704,7 @@
         <v>74.400000000000006</v>
       </c>
     </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
         <v>28</v>
       </c>
@@ -4929,14 +4735,14 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="53.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -4947,7 +4753,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -4961,7 +4767,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>13</v>
       </c>
@@ -4975,7 +4781,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>17</v>
       </c>
@@ -4989,7 +4795,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -5003,7 +4809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -5017,7 +4823,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>22</v>
       </c>
@@ -5031,7 +4837,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>23</v>
       </c>
@@ -5045,7 +4851,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
@@ -5056,7 +4862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
@@ -5070,12 +4876,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
@@ -5083,22 +4889,22 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="38.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:2" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>